<commit_message>
Completed Project Charter and Event Table
</commit_message>
<xml_diff>
--- a/Documentation/Event table.xlsx
+++ b/Documentation/Event table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROG3050\Project\Git\Grey-Cube-Development\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Level5\MSEnterprise\Grey-Cube-Development\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="299">
   <si>
     <t>Use Case#</t>
   </si>
@@ -750,9 +750,6 @@
     <t>Reports inquiry</t>
   </si>
   <si>
-    <t>Print a  report</t>
-  </si>
-  <si>
     <t>View a report</t>
   </si>
   <si>
@@ -774,21 +771,9 @@
     <t>Reset password</t>
   </si>
   <si>
-    <t>Over login attempts limit</t>
-  </si>
-  <si>
-    <t>Visitor tries to login account, but over the attempt limit</t>
-  </si>
-  <si>
-    <t>Check username and password in DB. Lock the member until member reset the password</t>
-  </si>
-  <si>
     <t>Send reset password page to member through registered email address</t>
   </si>
   <si>
-    <t>Add profile request</t>
-  </si>
-  <si>
     <t>Edit profile request</t>
   </si>
   <si>
@@ -810,33 +795,15 @@
     <t>Member wants to update password</t>
   </si>
   <si>
-    <t>Member wants to add shipping address</t>
-  </si>
-  <si>
-    <t>Member wants to delete shipping address</t>
-  </si>
-  <si>
     <t>Member wants to edit shipping address</t>
   </si>
   <si>
-    <t>Add shipping address</t>
-  </si>
-  <si>
-    <t>The new shipping address is added on DB, updated shipping address is displayed</t>
-  </si>
-  <si>
     <t>Edit shipping address</t>
   </si>
   <si>
     <t>Update the DB with the edited shipping address, updated shipping address is displayed</t>
   </si>
   <si>
-    <t>Delete shipping address</t>
-  </si>
-  <si>
-    <t>Delete the shipping address from DB, updated shipping addresss is displayed</t>
-  </si>
-  <si>
     <t>Member wants to add a new credit card</t>
   </si>
   <si>
@@ -873,18 +840,6 @@
     <t>Employee wants to approve game review</t>
   </si>
   <si>
-    <t>System creates a cart</t>
-  </si>
-  <si>
-    <t>Successful log in</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>A cart is created as part of the member's session</t>
-  </si>
-  <si>
     <t>Delete a game from cart in session</t>
   </si>
   <si>
@@ -946,6 +901,27 @@
   </si>
   <si>
     <t xml:space="preserve">Select games from DB where game name or category are the filtering content, returned games are displayed in list </t>
+  </si>
+  <si>
+    <t>Confirm change password</t>
+  </si>
+  <si>
+    <t>View a game details</t>
+  </si>
+  <si>
+    <t>Log Out</t>
+  </si>
+  <si>
+    <t>Member or Employee wants to log out</t>
+  </si>
+  <si>
+    <t>Logout Request</t>
+  </si>
+  <si>
+    <t>Member/Employee</t>
+  </si>
+  <si>
+    <t>session is cleared, visitor page is displayed</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1039,14 +1015,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1412,14 +1394,14 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="B4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1728,14 +1710,14 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1784,14 +1766,14 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1909,14 +1891,14 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -2057,14 +2039,14 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2113,14 +2095,14 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -2192,14 +2174,14 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -2271,13 +2253,13 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -2349,14 +2331,14 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -2474,13 +2456,13 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -2547,10 +2529,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2559,7 +2541,7 @@
     <col min="2" max="2" width="31.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="97.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="5"/>
@@ -2569,22 +2551,22 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2795,26 +2777,26 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="11" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2823,19 +2805,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>67</v>
+        <v>270</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>70</v>
+        <v>283</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>33</v>
@@ -2846,19 +2828,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>281</v>
+        <v>201</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>56</v>
+        <v>196</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>33</v>
@@ -2869,19 +2851,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>299</v>
+        <v>195</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>33</v>
@@ -2892,22 +2874,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>202</v>
+        <v>252</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>194</v>
+        <v>253</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>193</v>
+        <v>97</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>195</v>
+        <v>246</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2915,22 +2897,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>257</v>
+        <v>94</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>258</v>
+        <v>95</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>247</v>
+        <v>285</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2938,22 +2920,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>96</v>
+        <v>279</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2961,19 +2943,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>94</v>
+        <v>247</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>95</v>
+        <v>254</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>300</v>
+        <v>248</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>87</v>
@@ -2984,90 +2966,90 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>271</v>
+        <v>292</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>294</v>
+        <v>99</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>273</v>
+        <v>91</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="B20" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="B21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="B22" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3076,19 +3058,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>113</v>
+        <v>259</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>253</v>
+        <v>55</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>87</v>
@@ -3099,42 +3081,42 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>118</v>
+      <c r="F25" s="7" t="s">
+        <v>291</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>87</v>
@@ -3145,19 +3127,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>264</v>
+        <v>293</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>261</v>
+        <v>141</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>87</v>
@@ -3168,19 +3150,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>266</v>
+        <v>152</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>263</v>
+        <v>153</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>267</v>
+        <v>154</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>87</v>
@@ -3191,10 +3173,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>44</v>
@@ -3203,7 +3185,7 @@
         <v>87</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>87</v>
@@ -3214,19 +3196,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>128</v>
+        <v>267</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>55</v>
+        <v>265</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>130</v>
+        <v>266</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>87</v>
@@ -3237,42 +3219,42 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>139</v>
+        <v>44</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>306</v>
+      <c r="F31" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>87</v>
@@ -3283,19 +3265,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>38</v>
+        <v>280</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>87</v>
+        <v>282</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>279</v>
+        <v>159</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>87</v>
@@ -3306,10 +3288,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>55</v>
@@ -3318,7 +3300,7 @@
         <v>87</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>154</v>
+        <v>286</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>87</v>
@@ -3329,19 +3311,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>274</v>
+        <v>168</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>255</v>
+        <v>290</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>87</v>
@@ -3352,19 +3334,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>278</v>
+        <v>180</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>275</v>
+        <v>179</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>276</v>
+        <v>183</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>87</v>
@@ -3375,19 +3357,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>150</v>
+        <v>271</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>87</v>
@@ -3398,19 +3380,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>44</v>
+        <v>189</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>151</v>
+        <v>272</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>87</v>
@@ -3421,19 +3403,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>155</v>
+        <v>199</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>156</v>
+        <v>273</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>159</v>
+        <v>87</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>288</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>87</v>
@@ -3444,19 +3426,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>160</v>
+        <v>277</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>161</v>
+        <v>274</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>55</v>
+        <v>275</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>87</v>
@@ -3467,19 +3449,19 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>168</v>
+        <v>244</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>169</v>
+        <v>278</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>87</v>
@@ -3490,163 +3472,26 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>177</v>
+        <v>294</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>